<commit_message>
Refactor user data loading in DbSeeder
- Streamlined the user data loading process by integrating a new method for handling optional Stamp Image paths.
- Improved error handling for missing or empty data, providing clearer feedback on expected column headers.
- Enhanced the loading of stamp image bytes for better user image integration during seeding.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/MASTER - TOOL LIST.xlsx
+++ b/CNCToolingDatabase/Data/MASTER - TOOL LIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96491EAF-5211-42F6-AEF9-851408DD8E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98831436-A359-42F9-8356-54E7A1EA1B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="773" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="129">
   <si>
     <t>No.</t>
   </si>
@@ -314,12 +314,6 @@
     <t>A3389DPL-12</t>
   </si>
   <si>
-    <t>7792VXP06CA016Z2R140</t>
-  </si>
-  <si>
-    <t>7792VXD09WA032Z3R</t>
-  </si>
-  <si>
     <t>553060Z3.0-SIRON-A</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>7792VXD12-A052Z5R</t>
   </si>
   <si>
-    <t>7792VXD12-A080Z8R</t>
-  </si>
-  <si>
     <t>A3389DPL-6.1</t>
   </si>
   <si>
@@ -389,12 +380,6 @@
     <t>Drill Ø9.8</t>
   </si>
   <si>
-    <t>Facemill Ø16 High Feed</t>
-  </si>
-  <si>
-    <t>Facemill Ø32 High Feed</t>
-  </si>
-  <si>
     <t>Endmill Ø14 R0.0</t>
   </si>
   <si>
@@ -413,7 +398,34 @@
     <t>Endmill Ø12 R2.5</t>
   </si>
   <si>
-    <t>Facemill Ø80</t>
+    <t>6198036</t>
+  </si>
+  <si>
+    <t>Reamer Ø17.48</t>
+  </si>
+  <si>
+    <t>4BN0300MR020A,KC633M</t>
+  </si>
+  <si>
+    <t>Ballnose Ø3 R1.5</t>
+  </si>
+  <si>
+    <t>D9.567+/-0.002XCL30XOAL70XSHK10</t>
+  </si>
+  <si>
+    <t>Drill Ø9.567</t>
+  </si>
+  <si>
+    <t>HYP-HPO-GDS-3D-5.8X66X28X6</t>
+  </si>
+  <si>
+    <t>Drill Ø5.8</t>
+  </si>
+  <si>
+    <t>DLC-D10XR5XOAL100XCL18XSHK10X2FL</t>
+  </si>
+  <si>
+    <t>Mill Ø10 R5</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1568,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,16 +1601,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>7</v>
@@ -1736,7 +1748,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,7 +1838,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>89</v>
@@ -1850,7 +1862,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>90</v>
@@ -1876,10 +1888,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>57</v>
@@ -1902,13 +1914,13 @@
         <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H6" s="3">
         <v>75</v>
@@ -1926,10 +1938,10 @@
         <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>57</v>
@@ -1959,7 +1971,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2089,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H4" s="3">
         <v>55</v>
@@ -2153,7 +2165,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,10 +2229,10 @@
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>57</v>
@@ -2241,10 +2253,10 @@
         <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>57</v>
@@ -2267,10 +2279,10 @@
         <v>76</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>57</v>
@@ -2317,10 +2329,10 @@
         <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
@@ -2338,13 +2350,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>57</v>
@@ -2362,13 +2374,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>57</v>
@@ -2396,15 +2408,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84C940E-4B8F-41DF-9E6B-9ECB5611CCBD}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -2464,10 +2476,10 @@
         <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H2" s="3">
         <v>45</v>
@@ -2491,7 +2503,7 @@
         <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H3" s="3">
         <v>35</v>
@@ -2509,10 +2521,10 @@
         <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>57</v>
@@ -2561,10 +2573,10 @@
         <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
@@ -2593,7 +2605,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,13 +2719,13 @@
         <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H4" s="3">
         <v>55</v>
@@ -2731,10 +2743,10 @@
         <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>57</v>
@@ -2778,7 +2790,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Refactor ToolListEditorController for enhanced PDF export features and layout consistency
- Improved PDF export by refining the layout and positioning of tool details for better visibility.
- Updated header and table cell styles to ensure cohesive presentation across the document.
- Enhanced formatting of approval stamp items for improved aesthetics and clarity in the PDF export.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/MASTER - TOOL LIST.xlsx
+++ b/CNCToolingDatabase/Data/MASTER - TOOL LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98831436-A359-42F9-8356-54E7A1EA1B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492916B1-C874-4FAB-84E4-EAFAD3414745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="773" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -311,13 +311,7 @@
     <t>A3389DPL-9.8</t>
   </si>
   <si>
-    <t>A3389DPL-12</t>
-  </si>
-  <si>
     <t>553060Z3.0-SIRON-A</t>
-  </si>
-  <si>
-    <t>Drill Ø12</t>
   </si>
   <si>
     <t>553140Z3.0-SIRON-A</t>
@@ -1568,7 +1562,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,16 +1595,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>7</v>
@@ -1748,7 +1742,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,7 +1832,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>89</v>
@@ -1862,10 +1856,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>57</v>
@@ -1888,10 +1882,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>57</v>
@@ -1914,13 +1908,13 @@
         <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H6" s="3">
         <v>75</v>
@@ -1938,10 +1932,10 @@
         <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>57</v>
@@ -2089,7 +2083,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H4" s="3">
         <v>55</v>
@@ -2229,10 +2223,10 @@
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>57</v>
@@ -2253,10 +2247,10 @@
         <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>57</v>
@@ -2279,10 +2273,10 @@
         <v>76</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>57</v>
@@ -2329,10 +2323,10 @@
         <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
@@ -2350,13 +2344,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>57</v>
@@ -2374,13 +2368,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>57</v>
@@ -2473,13 +2467,13 @@
         <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H2" s="3">
         <v>45</v>
@@ -2503,7 +2497,7 @@
         <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H3" s="3">
         <v>35</v>
@@ -2521,10 +2515,10 @@
         <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>57</v>
@@ -2573,10 +2567,10 @@
         <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
@@ -2719,13 +2713,13 @@
         <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H4" s="3">
         <v>55</v>
@@ -2743,10 +2737,10 @@
         <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>57</v>
@@ -2790,7 +2784,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>53</v>

</xml_diff>